<commit_message>
Corrected spoofed and non-spoofed folder and updated contents of folders
</commit_message>
<xml_diff>
--- a/examples/ipv6/suppression-attack/CopyCat/CopyCat Processed Results/Backup files/Results Compiled - Backup.xlsx
+++ b/examples/ipv6/suppression-attack/CopyCat/CopyCat Processed Results/Backup files/Results Compiled - Backup.xlsx
@@ -4,12 +4,12 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Normal" sheetId="3" r:id="rId1"/>
-    <sheet name="Non-spoofed" sheetId="2" r:id="rId2"/>
-    <sheet name="Spoofed" sheetId="1" r:id="rId3"/>
+    <sheet name="Spoofed" sheetId="2" r:id="rId2"/>
+    <sheet name="Non-spoofed" sheetId="1" r:id="rId3"/>
   </sheets>
   <externalReferences>
     <externalReference r:id="rId4"/>
@@ -846,7 +846,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
@@ -1361,8 +1361,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X68"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="T68" sqref="T68"/>
+    <sheetView tabSelected="1" topLeftCell="A42" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J57" sqref="J57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2190,7 +2190,7 @@
       </c>
       <c r="O15">
         <f>T68</f>
-        <v>0.93367811667623324</v>
+        <v>0.93367811667623302</v>
       </c>
       <c r="S15" s="9" t="s">
         <v>19</v>
@@ -3229,7 +3229,7 @@
         <v>21</v>
       </c>
       <c r="T68" s="10">
-        <v>0.93367811667623324</v>
+        <v>0.93367811667623302</v>
       </c>
       <c r="U68" s="10" t="s">
         <v>21</v>

</xml_diff>